<commit_message>
- removed everything required for place categories. - added support for patch categories.
</commit_message>
<xml_diff>
--- a/tools/categories/category_list.xlsx
+++ b/tools/categories/category_list.xlsx
@@ -5,14 +5,15 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Proxibase\tools\categories\v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Proxibase\tools\categories\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4395" yWindow="285" windowWidth="27495" windowHeight="17880" tabRatio="654"/>
+    <workbookView xWindow="4395" yWindow="285" windowWidth="27495" windowHeight="17880" tabRatio="654" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="patches" sheetId="12" r:id="rId1"/>
+    <sheet name="patches_v2" sheetId="13" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="167">
   <si>
     <t>Pool Party</t>
   </si>
@@ -297,6 +298,234 @@
   </si>
   <si>
     <t>img_party.png</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>messages</t>
+  </si>
+  <si>
+    <t>social event</t>
+  </si>
+  <si>
+    <t>meeting</t>
+  </si>
+  <si>
+    <t>trip</t>
+  </si>
+  <si>
+    <t>reviews</t>
+  </si>
+  <si>
+    <t>tips</t>
+  </si>
+  <si>
+    <t>club</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>interest</t>
+  </si>
+  <si>
+    <t>stash</t>
+  </si>
+  <si>
+    <t>cache</t>
+  </si>
+  <si>
+    <t>chat</t>
+  </si>
+  <si>
+    <t>discussion</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>employees</t>
+  </si>
+  <si>
+    <t>vendors</t>
+  </si>
+  <si>
+    <t>partners</t>
+  </si>
+  <si>
+    <t>mvps</t>
+  </si>
+  <si>
+    <t>fans</t>
+  </si>
+  <si>
+    <t>treasure</t>
+  </si>
+  <si>
+    <t>Cache</t>
+  </si>
+  <si>
+    <t>concert</t>
+  </si>
+  <si>
+    <t>party</t>
+  </si>
+  <si>
+    <t>reunion</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>training</t>
+  </si>
+  <si>
+    <t>workshop</t>
+  </si>
+  <si>
+    <t>game</t>
+  </si>
+  <si>
+    <t>festival</t>
+  </si>
+  <si>
+    <t>fair</t>
+  </si>
+  <si>
+    <t>dinner</t>
+  </si>
+  <si>
+    <t>networking</t>
+  </si>
+  <si>
+    <t>seminar</t>
+  </si>
+  <si>
+    <t>talk</t>
+  </si>
+  <si>
+    <t>sports</t>
+  </si>
+  <si>
+    <t>performance</t>
+  </si>
+  <si>
+    <t>Networking</t>
+  </si>
+  <si>
+    <t>Party</t>
+  </si>
+  <si>
+    <t>Reunion</t>
+  </si>
+  <si>
+    <t>Seminar</t>
+  </si>
+  <si>
+    <t>Sports</t>
+  </si>
+  <si>
+    <t>Talk</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Treasure</t>
+  </si>
+  <si>
+    <t>Workshop</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>Social</t>
+  </si>
+  <si>
+    <t>Stash</t>
+  </si>
+  <si>
+    <t>Tips</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Trip</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>Chat</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Meeting</t>
+  </si>
+  <si>
+    <t>Club</t>
+  </si>
+  <si>
+    <t>Concert</t>
+  </si>
+  <si>
+    <t>Dinner</t>
+  </si>
+  <si>
+    <t>Discussion</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Fair</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>Fan</t>
+  </si>
+  <si>
+    <t>Festival</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Interest</t>
+  </si>
+  <si>
+    <t>Messages</t>
+  </si>
+  <si>
+    <t>MVP</t>
+  </si>
+  <si>
+    <t>Reviews</t>
+  </si>
+  <si>
+    <t>show</t>
+  </si>
+  <si>
+    <t>Show</t>
   </si>
 </sst>
 </file>
@@ -376,7 +605,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -385,13 +614,99 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -491,8 +806,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="patch_cat_list" displayName="patch_cat_list" ref="A1:E42" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="patch_cat_list" displayName="patch_cat_list" ref="A1:E42" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:E42"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="id" dataDxfId="11"/>
+    <tableColumn id="2" name="name" dataDxfId="10"/>
+    <tableColumn id="3" name="parent_id" dataDxfId="9"/>
+    <tableColumn id="4" name="parent_name" dataDxfId="8"/>
+    <tableColumn id="5" name="icon" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="patch_cat_list2" displayName="patch_cat_list2" ref="A1:E46" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E46"/>
+  <sortState ref="A2:E46">
+    <sortCondition ref="A1:A46"/>
+  </sortState>
   <tableColumns count="5">
     <tableColumn id="1" name="id" dataDxfId="4"/>
     <tableColumn id="2" name="name" dataDxfId="3"/>
@@ -828,7 +1160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -1571,4 +1903,585 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="20" width="10" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="11" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- added patch categories.
</commit_message>
<xml_diff>
--- a/tools/categories/category_list.xlsx
+++ b/tools/categories/category_list.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="181">
   <si>
     <t>Pool Party</t>
   </si>
@@ -336,9 +336,6 @@
     <t>stash</t>
   </si>
   <si>
-    <t>cache</t>
-  </si>
-  <si>
     <t>chat</t>
   </si>
   <si>
@@ -366,9 +363,6 @@
     <t>treasure</t>
   </si>
   <si>
-    <t>Cache</t>
-  </si>
-  <si>
     <t>concert</t>
   </si>
   <si>
@@ -526,6 +520,54 @@
   </si>
   <si>
     <t>Show</t>
+  </si>
+  <si>
+    <t>tailgate</t>
+  </si>
+  <si>
+    <t>Tailgate</t>
+  </si>
+  <si>
+    <t>rehearsal</t>
+  </si>
+  <si>
+    <t>Rehearsal</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>happy hour</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>lunch</t>
+  </si>
+  <si>
+    <t>breakfast</t>
+  </si>
+  <si>
+    <t>Happy Hour</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Lunch</t>
+  </si>
+  <si>
+    <t>Breakfast</t>
+  </si>
+  <si>
+    <t>geocache</t>
+  </si>
+  <si>
+    <t>Geocache</t>
   </si>
 </sst>
 </file>
@@ -820,10 +862,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="patch_cat_list2" displayName="patch_cat_list2" ref="A1:E46" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E46"/>
-  <sortState ref="A2:E46">
-    <sortCondition ref="A1:A46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="patch_cat_list2" displayName="patch_cat_list2" ref="A1:E54" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E54"/>
+  <sortState ref="A2:E54">
+    <sortCondition ref="A1:A54"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" name="id" dataDxfId="4"/>
@@ -1907,10 +1949,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1955,22 +1997,24 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>113</v>
-      </c>
+      <c r="A3" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
       <c r="E3" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>87</v>
@@ -1978,10 +2022,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -1994,7 +2038,7 @@
         <v>98</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>87</v>
@@ -2002,10 +2046,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -2041,10 +2085,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>123</v>
+        <v>170</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -2053,127 +2097,129 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>152</v>
-      </c>
+      <c r="A11" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
       <c r="E11" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
       <c r="E14" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>155</v>
-      </c>
+      <c r="A15" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
       <c r="E15" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+      <c r="A17" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="E17" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="B20" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>99</v>
+      <c r="A21" s="3" t="s">
+        <v>179</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>87</v>
@@ -2181,45 +2227,45 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>110</v>
-      </c>
       <c r="B25" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>87</v>
@@ -2227,58 +2273,58 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>124</v>
+        <v>173</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>129</v>
+        <v>177</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>20</v>
+        <v>146</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
+      <c r="B29" s="2" t="s">
+        <v>161</v>
+      </c>
       <c r="E29" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -2287,142 +2333,146 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A31" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
       <c r="E31" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
+      <c r="A32" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="E32" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>96</v>
+      <c r="A33" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>164</v>
+        <v>136</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>132</v>
+      <c r="A34" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>165</v>
+        <v>126</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>166</v>
+        <v>143</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>139</v>
-      </c>
+      <c r="A36" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
       <c r="E36" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
+      <c r="A37" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="E37" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>140</v>
-      </c>
+      <c r="A38" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
       <c r="E38" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>142</v>
-      </c>
+      <c r="A41" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
       <c r="E41" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
@@ -2431,50 +2481,146 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
+      <c r="A43" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>137</v>
+      </c>
       <c r="E43" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>143</v>
-      </c>
+      <c r="A44" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
       <c r="E44" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>108</v>
+      <c r="A45" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>119</v>
+        <v>165</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="2" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- added new patch types: gossip, hangout
</commit_message>
<xml_diff>
--- a/tools/categories/category_list.xlsx
+++ b/tools/categories/category_list.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="185">
   <si>
     <t>Pool Party</t>
   </si>
@@ -568,6 +568,18 @@
   </si>
   <si>
     <t>Geocache</t>
+  </si>
+  <si>
+    <t>gossip</t>
+  </si>
+  <si>
+    <t>Gossip</t>
+  </si>
+  <si>
+    <t>hangout</t>
+  </si>
+  <si>
+    <t>Hangout</t>
   </si>
 </sst>
 </file>
@@ -862,10 +874,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="patch_cat_list2" displayName="patch_cat_list2" ref="A1:E54" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E54"/>
-  <sortState ref="A2:E54">
-    <sortCondition ref="A1:A54"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="patch_cat_list2" displayName="patch_cat_list2" ref="A1:E56" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E56"/>
+  <sortState ref="A2:E56">
+    <sortCondition ref="A1:A56"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" name="id" dataDxfId="4"/>
@@ -1949,10 +1961,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2226,105 +2238,107 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="E23" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B25" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
       <c r="E26" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>160</v>
+      <c r="A28" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>177</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>109</v>
+      <c r="A29" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>127</v>
+      <c r="A30" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>160</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -2333,133 +2347,133 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B33" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="E34" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+      <c r="E35" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B36" s="6" t="s">
         <v>128</v>
-      </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>69</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A37" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
       <c r="E37" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>167</v>
+        <v>68</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>168</v>
+        <v>69</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
+      <c r="A39" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="E39" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>162</v>
-      </c>
+      <c r="A40" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
       <c r="E40" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
@@ -2468,48 +2482,48 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
+      <c r="A42" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="E42" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>137</v>
-      </c>
+      <c r="A43" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
       <c r="E43" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>131</v>
+        <v>164</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>89</v>
@@ -2517,110 +2531,134 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>165</v>
+        <v>125</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B49" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E48" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="E50" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E49" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+      <c r="E51" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B52" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B53" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="E54" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
+      <c r="E55" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B56" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="2" t="s">
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="2" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- added patch type: holiday
</commit_message>
<xml_diff>
--- a/tools/categories/category_list.xlsx
+++ b/tools/categories/category_list.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="187">
   <si>
     <t>Pool Party</t>
   </si>
@@ -580,6 +580,12 @@
   </si>
   <si>
     <t>Hangout</t>
+  </si>
+  <si>
+    <t>holiday</t>
+  </si>
+  <si>
+    <t>Holiday</t>
   </si>
 </sst>
 </file>
@@ -874,10 +880,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="patch_cat_list2" displayName="patch_cat_list2" ref="A1:E56" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E56"/>
-  <sortState ref="A2:E56">
-    <sortCondition ref="A1:A56"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="patch_cat_list2" displayName="patch_cat_list2" ref="A1:E57" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E57"/>
+  <sortState ref="A2:E57">
+    <sortCondition ref="A1:A57"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" name="id" dataDxfId="4"/>
@@ -1961,10 +1967,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2288,94 +2294,94 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>87</v>
+      <c r="A26" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="E28" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B29" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="E30" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B31" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
       <c r="E32" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>172</v>
+        <v>122</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>176</v>
+        <v>127</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -2384,46 +2390,46 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="E35" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="E36" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B37" s="6" t="s">
         <v>128</v>
-      </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>143</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -2433,47 +2439,47 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>68</v>
+        <v>126</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>69</v>
+        <v>143</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
       <c r="E40" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>114</v>
+        <v>167</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>129</v>
+        <v>168</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
@@ -2482,35 +2488,35 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
       <c r="E43" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>163</v>
+        <v>123</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>164</v>
+        <v>130</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
@@ -2519,146 +2525,159 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
+      <c r="E46" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B47" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E47" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
       <c r="E48" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>124</v>
+        <v>165</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>132</v>
+        <v>166</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>139</v>
-      </c>
+      <c r="A50" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
       <c r="E50" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E51" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
+      <c r="E52" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B53" s="7" t="s">
         <v>133</v>
-      </c>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>134</v>
       </c>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E54" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+      <c r="E55" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
+      <c r="E56" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B57" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="2" t="s">
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="2" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>